<commit_message>
fixed bug in xlsx
</commit_message>
<xml_diff>
--- a/DATA/Protest is SA   SAS rules V2 - Separated.xlsx
+++ b/DATA/Protest is SA   SAS rules V2 - Separated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2022\Sem 1\ELEN4002 Capstone Project\Code\Team-Riot\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FD2A24-BD12-4EC6-9126-E5BFED01452A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6909657C-631B-4FCE-9D95-3EA1BED82CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4016,8 +4016,8 @@
   </sheetPr>
   <dimension ref="A1:F987"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Scraped, processed for fmf
</commit_message>
<xml_diff>
--- a/DATA/Protest is SA   SAS rules V2 - Separated.xlsx
+++ b/DATA/Protest is SA   SAS rules V2 - Separated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2022\Sem 1\ELEN4002 Capstone Project\Code\Team-Riot\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA39F56-F4EA-4F4E-BA1B-3266A5542CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB002A3A-2171-47E0-BD29-AC221DFC3FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1491,10 +1491,10 @@
     <t xml:space="preserve">boycot,boycott, ban </t>
   </si>
   <si>
-    <t>ANC,Congress, DA , EFF ,IFP,NFP, cope,cope ,UDM,SACP,ACDP</t>
-  </si>
-  <si>
     <t>Embassy,solidarily with the people of, war ,the situation in</t>
+  </si>
+  <si>
+    <t>ANC,Congress,IFP,NFP,UDM,SACP,ACDP</t>
   </si>
 </sst>
 </file>
@@ -4026,8 +4026,8 @@
   </sheetPr>
   <dimension ref="A1:F979"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4306,7 +4306,7 @@
         <v>264</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="24" t="s">
@@ -5242,7 +5242,7 @@
         <v>135</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="24" t="s">

</xml_diff>